<commit_message>
Test-9 for NN (nextyear)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-9.xlsx
+++ b/migforecasting/underground/test-9.xlsx
@@ -121,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -131,9 +131,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2698,7 +2695,7 @@
   <dimension ref="C4:AA66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB11" sqref="AB11"/>
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2807,8 +2804,12 @@
       <c r="Y7" s="2">
         <v>1</v>
       </c>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
+      <c r="Z7" s="3">
+        <v>560.50998950074211</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>1275.600167235162</v>
+      </c>
     </row>
     <row r="8" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
@@ -2844,8 +2845,12 @@
       <c r="Y8" s="2">
         <v>2</v>
       </c>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
+      <c r="Z8" s="3">
+        <v>522.05038851027052</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>1245.00450099573</v>
+      </c>
     </row>
     <row r="9" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
@@ -2881,8 +2886,12 @@
       <c r="Y9" s="2">
         <v>3</v>
       </c>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="5"/>
+      <c r="Z9" s="3">
+        <v>510.54175828544771</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>1224.0457560982541</v>
+      </c>
     </row>
     <row r="10" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
@@ -2918,8 +2927,12 @@
       <c r="Y10" s="2">
         <v>4</v>
       </c>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
+      <c r="Z10" s="3">
+        <v>594.83201247958345</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>1250.881080885373</v>
+      </c>
     </row>
     <row r="11" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
@@ -2955,8 +2968,12 @@
       <c r="Y11" s="2">
         <v>5</v>
       </c>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="5"/>
+      <c r="Z11" s="3">
+        <v>533.71593172848497</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>1233.518200058767</v>
+      </c>
     </row>
     <row r="12" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
@@ -2992,8 +3009,12 @@
       <c r="Y12" s="2">
         <v>6</v>
       </c>
-      <c r="Z12" s="5"/>
-      <c r="AA12" s="5"/>
+      <c r="Z12" s="3">
+        <v>490.57063055947663</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>1424.9429228418469</v>
+      </c>
     </row>
     <row r="13" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
@@ -3029,8 +3050,12 @@
       <c r="Y13" s="2">
         <v>7</v>
       </c>
-      <c r="Z13" s="5"/>
-      <c r="AA13" s="5"/>
+      <c r="Z13" s="3">
+        <v>500.95261468811299</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>1317.0755869606271</v>
+      </c>
     </row>
     <row r="14" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
@@ -3066,8 +3091,12 @@
       <c r="Y14" s="2">
         <v>8</v>
       </c>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="5"/>
+      <c r="Z14" s="3">
+        <v>526.10675567673206</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>1268.094857237646</v>
+      </c>
     </row>
     <row r="15" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
@@ -3103,8 +3132,12 @@
       <c r="Y15" s="2">
         <v>9</v>
       </c>
-      <c r="Z15" s="5"/>
-      <c r="AA15" s="5"/>
+      <c r="Z15" s="3">
+        <v>493.94392799948582</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>1352.9965724416379</v>
+      </c>
     </row>
     <row r="16" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
@@ -3140,8 +3173,12 @@
       <c r="Y16" s="2">
         <v>10</v>
       </c>
-      <c r="Z16" s="5"/>
-      <c r="AA16" s="5"/>
+      <c r="Z16" s="3">
+        <v>487.81024884027039</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>1309.1864162922529</v>
+      </c>
     </row>
     <row r="17" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
@@ -3177,8 +3214,12 @@
       <c r="Y17" s="2">
         <v>11</v>
       </c>
-      <c r="Z17" s="5"/>
-      <c r="AA17" s="5"/>
+      <c r="Z17" s="3">
+        <v>501.7510623320257</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>1256.8473536241429</v>
+      </c>
     </row>
     <row r="18" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
@@ -3214,8 +3255,12 @@
       <c r="Y18" s="2">
         <v>12</v>
       </c>
-      <c r="Z18" s="5"/>
-      <c r="AA18" s="5"/>
+      <c r="Z18" s="3">
+        <v>601.22116389570601</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>1327.9264803926901</v>
+      </c>
     </row>
     <row r="19" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
@@ -3251,8 +3296,12 @@
       <c r="Y19" s="2">
         <v>13</v>
       </c>
-      <c r="Z19" s="5"/>
-      <c r="AA19" s="5"/>
+      <c r="Z19" s="3">
+        <v>565.4341859150062</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>1135.0631737094229</v>
+      </c>
     </row>
     <row r="20" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
@@ -3288,8 +3337,12 @@
       <c r="Y20" s="2">
         <v>14</v>
       </c>
-      <c r="Z20" s="5"/>
-      <c r="AA20" s="5"/>
+      <c r="Z20" s="3">
+        <v>608.49863593354053</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>1204.007012169282</v>
+      </c>
     </row>
     <row r="21" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
@@ -3325,8 +3378,12 @@
       <c r="Y21" s="2">
         <v>15</v>
       </c>
-      <c r="Z21" s="5"/>
-      <c r="AA21" s="5"/>
+      <c r="Z21" s="3">
+        <v>521.39625719769197</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>1335.897831061056</v>
+      </c>
     </row>
     <row r="22" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
@@ -3362,8 +3419,12 @@
       <c r="Y22" s="2">
         <v>16</v>
       </c>
-      <c r="Z22" s="5"/>
-      <c r="AA22" s="5"/>
+      <c r="Z22" s="3">
+        <v>524.26255120630321</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>1399.736875125539</v>
+      </c>
     </row>
     <row r="23" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
@@ -3399,8 +3460,12 @@
       <c r="Y23" s="2">
         <v>17</v>
       </c>
-      <c r="Z23" s="5"/>
-      <c r="AA23" s="5"/>
+      <c r="Z23" s="3">
+        <v>544.10427197046988</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>1292.224007560751</v>
+      </c>
     </row>
     <row r="24" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
@@ -3436,8 +3501,12 @@
       <c r="Y24" s="2">
         <v>18</v>
       </c>
-      <c r="Z24" s="5"/>
-      <c r="AA24" s="5"/>
+      <c r="Z24" s="3">
+        <v>518.69560857377508</v>
+      </c>
+      <c r="AA24" s="3">
+        <v>1217.131283365979</v>
+      </c>
     </row>
     <row r="25" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
@@ -3473,8 +3542,12 @@
       <c r="Y25" s="2">
         <v>19</v>
       </c>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="5"/>
+      <c r="Z25" s="3">
+        <v>496.69156082074068</v>
+      </c>
+      <c r="AA25" s="3">
+        <v>1235.834797935581</v>
+      </c>
     </row>
     <row r="26" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
@@ -3510,8 +3583,12 @@
       <c r="Y26" s="2">
         <v>20</v>
       </c>
-      <c r="Z26" s="5"/>
-      <c r="AA26" s="5"/>
+      <c r="Z26" s="3">
+        <v>471.4935830244371</v>
+      </c>
+      <c r="AA26" s="3">
+        <v>1343.899372083657</v>
+      </c>
     </row>
     <row r="27" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
@@ -3545,8 +3622,8 @@
         <v>1242.798067341434</v>
       </c>
       <c r="Y27" s="2"/>
-      <c r="Z27" s="5"/>
-      <c r="AA27" s="4"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
     </row>
     <row r="28" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
@@ -3582,13 +3659,13 @@
       <c r="Y28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Z28" s="5" t="e">
+      <c r="Z28" s="3">
         <f>AVERAGE(Z7:Z26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA28" s="5" t="e">
+        <v>528.72915695691518</v>
+      </c>
+      <c r="AA28" s="3">
         <f>AVERAGE(AA7:AA26)</f>
-        <v>#DIV/0!</v>
+        <v>1282.4957124037701</v>
       </c>
     </row>
     <row r="29" spans="3:27" x14ac:dyDescent="0.25">
@@ -3625,13 +3702,13 @@
       <c r="Y29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Z29" s="5" t="e">
+      <c r="Z29" s="3">
         <f>_xlfn.STDEV.S(Z7:Z26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AA29" s="5" t="e">
+        <v>39.273108587288675</v>
+      </c>
+      <c r="AA29" s="3">
         <f>_xlfn.STDEV.S(AA7:AA26)</f>
-        <v>#DIV/0!</v>
+        <v>70.028430793437636</v>
       </c>
     </row>
     <row r="30" spans="3:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Test-10 for tree (this, next)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-9.xlsx
+++ b/migforecasting/underground/test-9.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ThisYear" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -303,7 +302,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -424,7 +422,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -567,7 +564,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2694,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4:O59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>